<commit_message>
0705 commit,Confidence interval,match with colab
</commit_message>
<xml_diff>
--- a/miangyang_aircon_June.xlsx
+++ b/miangyang_aircon_June.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qlvzy\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qlvzy\PycharmProjects\nenghaoyichang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A7FC10-60A4-471C-9E92-AA67662F4B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3C5A30-43B7-4E63-AE7B-4B743B921858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2156,6 +2156,4922 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$A$17:$A$688</c:f>
+              <c:strCache>
+                <c:ptCount val="672"/>
+                <c:pt idx="0">
+                  <c:v>2022-06-01 15:00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2022-06-01 16:00</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2022-06-01 17:00</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2022-06-01 18:00</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2022-06-01 19:00</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2022-06-01 20:00</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2022-06-01 21:00</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2022-06-01 22:00</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2022-06-01 23:00</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2022-06-02 00:00</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2022-06-02 01:00</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2022-06-02 02:00</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2022-06-02 03:00</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2022-06-02 04:00</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2022-06-02 05:00</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2022-06-02 06:00</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2022-06-02 07:00</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2022-06-02 08:00</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2022-06-02 09:00</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2022-06-02 10:00</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2022-06-02 11:00</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2022-06-02 12:00</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2022-06-02 13:00</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2022-06-02 14:00</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2022-06-02 15:00</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2022-06-02 16:00</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2022-06-02 17:00</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2022-06-02 18:00</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2022-06-02 19:00</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2022-06-02 20:00</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2022-06-02 21:00</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2022-06-02 22:00</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2022-06-02 23:00</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2022-06-03 00:00</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2022-06-03 01:00</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2022-06-03 02:00</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2022-06-03 03:00</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2022-06-03 04:00</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2022-06-03 05:00</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2022-06-03 06:00</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2022-06-03 07:00</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2022-06-03 08:00</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2022-06-03 09:00</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2022-06-03 10:00</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2022-06-03 11:00</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2022-06-03 12:00</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2022-06-03 13:00</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2022-06-03 14:00</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2022-06-03 15:00</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2022-06-03 16:00</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2022-06-03 17:00</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2022-06-03 18:00</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2022-06-03 19:00</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2022-06-03 20:00</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2022-06-03 21:00</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2022-06-03 22:00</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2022-06-03 23:00</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2022-06-04 00:00</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2022-06-04 01:00</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2022-06-04 02:00</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2022-06-04 03:00</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2022-06-04 04:00</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2022-06-04 05:00</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2022-06-04 06:00</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2022-06-04 07:00</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2022-06-04 08:00</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2022-06-04 09:00</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2022-06-04 10:00</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2022-06-04 11:00</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2022-06-04 12:00</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2022-06-04 13:00</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2022-06-04 14:00</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2022-06-04 15:00</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2022-06-04 16:00</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2022-06-04 17:00</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2022-06-04 18:00</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2022-06-04 19:00</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2022-06-04 20:00</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2022-06-04 21:00</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2022-06-04 22:00</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2022-06-04 23:00</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2022-06-05 00:00</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2022-06-05 01:00</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2022-06-05 02:00</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2022-06-05 03:00</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2022-06-05 04:00</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2022-06-05 05:00</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2022-06-05 06:00</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2022-06-05 07:00</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2022-06-05 08:00</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2022-06-05 09:00</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2022-06-05 10:00</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2022-06-05 11:00</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2022-06-05 12:00</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2022-06-05 13:00</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2022-06-05 14:00</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2022-06-05 15:00</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2022-06-05 16:00</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2022-06-05 17:00</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2022-06-05 18:00</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2022-06-05 19:00</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2022-06-05 20:00</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2022-06-05 21:00</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>2022-06-05 22:00</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2022-06-05 23:00</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>2022-06-06 00:00</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>2022-06-06 01:00</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>2022-06-06 02:00</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>2022-06-06 03:00</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>2022-06-06 04:00</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>2022-06-06 05:00</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>2022-06-06 06:00</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>2022-06-06 07:00</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>2022-06-06 08:00</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>2022-06-06 09:00</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>2022-06-06 10:00</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>2022-06-06 11:00</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>2022-06-06 12:00</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>2022-06-06 13:00</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>2022-06-06 14:00</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>2022-06-06 15:00</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>2022-06-06 16:00</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>2022-06-06 17:00</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>2022-06-06 18:00</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>2022-06-06 19:00</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>2022-06-06 20:00</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>2022-06-06 21:00</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>2022-06-06 22:00</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>2022-06-06 23:00</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>2022-06-07 00:00</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>2022-06-07 01:00</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>2022-06-07 02:00</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>2022-06-07 03:00</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>2022-06-07 04:00</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>2022-06-07 05:00</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>2022-06-07 06:00</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>2022-06-07 07:00</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>2022-06-07 08:00</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>2022-06-07 09:00</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>2022-06-07 10:00</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>2022-06-07 11:00</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>2022-06-07 12:00</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>2022-06-07 13:00</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>2022-06-07 14:00</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>2022-06-07 15:00</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>2022-06-07 16:00</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>2022-06-07 17:00</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>2022-06-07 18:00</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>2022-06-07 19:00</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>2022-06-07 20:00</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>2022-06-07 21:00</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>2022-06-07 22:00</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>2022-06-07 23:00</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>2022-06-08 00:00</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>2022-06-08 01:00</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>2022-06-08 02:00</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>2022-06-08 03:00</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>2022-06-08 04:00</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>2022-06-08 05:00</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>2022-06-08 06:00</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>2022-06-08 07:00</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>2022-06-08 08:00</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>2022-06-08 09:00</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>2022-06-08 10:00</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>2022-06-08 11:00</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>2022-06-08 12:00</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>2022-06-08 13:00</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>2022-06-08 14:00</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>2022-06-08 15:00</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>2022-06-08 16:00</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>2022-06-08 17:00</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>2022-06-08 18:00</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>2022-06-08 19:00</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>2022-06-08 20:00</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>2022-06-08 21:00</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>2022-06-08 22:00</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>2022-06-08 23:00</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>2022-06-09 00:00</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>2022-06-09 01:00</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>2022-06-09 02:00</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>2022-06-09 03:00</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>2022-06-09 04:00</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>2022-06-09 05:00</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>2022-06-09 06:00</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>2022-06-09 07:00</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>2022-06-09 08:00</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>2022-06-09 09:00</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>2022-06-09 10:00</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>2022-06-09 11:00</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>2022-06-09 12:00</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>2022-06-09 13:00</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>2022-06-09 14:00</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>2022-06-09 15:00</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>2022-06-09 16:00</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>2022-06-09 17:00</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>2022-06-09 18:00</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>2022-06-09 19:00</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>2022-06-09 20:00</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>2022-06-09 21:00</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>2022-06-09 22:00</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>2022-06-09 23:00</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>2022-06-10 00:00</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>2022-06-10 01:00</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>2022-06-10 02:00</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>2022-06-10 03:00</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>2022-06-10 04:00</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>2022-06-10 05:00</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>2022-06-10 06:00</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>2022-06-10 07:00</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>2022-06-10 08:00</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>2022-06-10 09:00</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>2022-06-10 10:00</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>2022-06-10 11:00</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>2022-06-10 12:00</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>2022-06-10 13:00</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>2022-06-10 14:00</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>2022-06-10 15:00</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>2022-06-10 16:00</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>2022-06-10 17:00</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>2022-06-10 18:00</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>2022-06-10 19:00</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>2022-06-10 20:00</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>2022-06-10 21:00</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>2022-06-10 22:00</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>2022-06-10 23:00</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>2022-06-11 00:00</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>2022-06-11 01:00</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>2022-06-11 02:00</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>2022-06-11 03:00</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>2022-06-11 04:00</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>2022-06-11 05:00</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>2022-06-11 06:00</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>2022-06-11 07:00</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>2022-06-11 08:00</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>2022-06-11 09:00</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>2022-06-11 10:00</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>2022-06-11 11:00</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>2022-06-11 12:00</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>2022-06-11 13:00</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>2022-06-11 14:00</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>2022-06-11 15:00</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>2022-06-11 16:00</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>2022-06-11 17:00</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>2022-06-11 18:00</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>2022-06-11 19:00</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>2022-06-11 20:00</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>2022-06-11 21:00</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>2022-06-11 22:00</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>2022-06-11 23:00</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>2022-06-12 00:00</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>2022-06-12 01:00</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>2022-06-12 02:00</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>2022-06-12 03:00</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>2022-06-12 04:00</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>2022-06-12 05:00</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>2022-06-12 06:00</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>2022-06-12 07:00</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>2022-06-12 08:00</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>2022-06-12 09:00</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>2022-06-12 10:00</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>2022-06-12 11:00</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>2022-06-12 12:00</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>2022-06-12 13:00</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>2022-06-12 14:00</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>2022-06-12 15:00</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>2022-06-12 16:00</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>2022-06-12 17:00</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>2022-06-12 18:00</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>2022-06-12 19:00</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>2022-06-12 20:00</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>2022-06-12 21:00</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>2022-06-12 22:00</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>2022-06-12 23:00</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>2022-06-13 00:00</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>2022-06-13 01:00</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>2022-06-13 02:00</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>2022-06-13 03:00</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>2022-06-13 04:00</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>2022-06-13 05:00</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>2022-06-13 06:00</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>2022-06-13 07:00</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>2022-06-13 08:00</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>2022-06-13 09:00</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>2022-06-13 10:00</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>2022-06-13 11:00</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>2022-06-13 12:00</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>2022-06-13 13:00</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>2022-06-13 14:00</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>2022-06-13 15:00</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>2022-06-13 16:00</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>2022-06-13 17:00</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>2022-06-13 18:00</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>2022-06-13 19:00</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>2022-06-13 20:00</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>2022-06-13 21:00</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>2022-06-13 22:00</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>2022-06-13 23:00</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>2022-06-14 00:00</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>2022-06-14 01:00</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>2022-06-14 02:00</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>2022-06-14 03:00</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>2022-06-14 04:00</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>2022-06-14 05:00</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>2022-06-14 06:00</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>2022-06-14 07:00</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>2022-06-14 08:00</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>2022-06-14 09:00</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>2022-06-14 10:00</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>2022-06-14 11:00</c:v>
+                </c:pt>
+                <c:pt idx="309">
+                  <c:v>2022-06-14 12:00</c:v>
+                </c:pt>
+                <c:pt idx="310">
+                  <c:v>2022-06-14 13:00</c:v>
+                </c:pt>
+                <c:pt idx="311">
+                  <c:v>2022-06-14 14:00</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>2022-06-14 15:00</c:v>
+                </c:pt>
+                <c:pt idx="313">
+                  <c:v>2022-06-14 16:00</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>2022-06-14 17:00</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>2022-06-14 18:00</c:v>
+                </c:pt>
+                <c:pt idx="316">
+                  <c:v>2022-06-14 19:00</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>2022-06-14 20:00</c:v>
+                </c:pt>
+                <c:pt idx="318">
+                  <c:v>2022-06-14 21:00</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>2022-06-14 22:00</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>2022-06-14 23:00</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>2022-06-15 00:00</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>2022-06-15 01:00</c:v>
+                </c:pt>
+                <c:pt idx="323">
+                  <c:v>2022-06-15 02:00</c:v>
+                </c:pt>
+                <c:pt idx="324">
+                  <c:v>2022-06-15 03:00</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>2022-06-15 04:00</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>2022-06-15 05:00</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>2022-06-15 06:00</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>2022-06-15 07:00</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>2022-06-15 08:00</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>2022-06-15 09:00</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>2022-06-15 10:00</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>2022-06-15 11:00</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>2022-06-15 12:00</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>2022-06-15 13:00</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>2022-06-15 14:00</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>2022-06-15 15:00</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>2022-06-15 16:00</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>2022-06-15 17:00</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>2022-06-15 18:00</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>2022-06-15 19:00</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>2022-06-15 20:00</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>2022-06-15 21:00</c:v>
+                </c:pt>
+                <c:pt idx="343">
+                  <c:v>2022-06-15 22:00</c:v>
+                </c:pt>
+                <c:pt idx="344">
+                  <c:v>2022-06-15 23:00</c:v>
+                </c:pt>
+                <c:pt idx="345">
+                  <c:v>2022-06-16 00:00</c:v>
+                </c:pt>
+                <c:pt idx="346">
+                  <c:v>2022-06-16 01:00</c:v>
+                </c:pt>
+                <c:pt idx="347">
+                  <c:v>2022-06-16 02:00</c:v>
+                </c:pt>
+                <c:pt idx="348">
+                  <c:v>2022-06-16 03:00</c:v>
+                </c:pt>
+                <c:pt idx="349">
+                  <c:v>2022-06-16 04:00</c:v>
+                </c:pt>
+                <c:pt idx="350">
+                  <c:v>2022-06-16 05:00</c:v>
+                </c:pt>
+                <c:pt idx="351">
+                  <c:v>2022-06-16 06:00</c:v>
+                </c:pt>
+                <c:pt idx="352">
+                  <c:v>2022-06-16 07:00</c:v>
+                </c:pt>
+                <c:pt idx="353">
+                  <c:v>2022-06-16 08:00</c:v>
+                </c:pt>
+                <c:pt idx="354">
+                  <c:v>2022-06-16 09:00</c:v>
+                </c:pt>
+                <c:pt idx="355">
+                  <c:v>2022-06-16 10:00</c:v>
+                </c:pt>
+                <c:pt idx="356">
+                  <c:v>2022-06-16 11:00</c:v>
+                </c:pt>
+                <c:pt idx="357">
+                  <c:v>2022-06-16 12:00</c:v>
+                </c:pt>
+                <c:pt idx="358">
+                  <c:v>2022-06-16 13:00</c:v>
+                </c:pt>
+                <c:pt idx="359">
+                  <c:v>2022-06-16 14:00</c:v>
+                </c:pt>
+                <c:pt idx="360">
+                  <c:v>2022-06-16 15:00</c:v>
+                </c:pt>
+                <c:pt idx="361">
+                  <c:v>2022-06-16 16:00</c:v>
+                </c:pt>
+                <c:pt idx="362">
+                  <c:v>2022-06-16 17:00</c:v>
+                </c:pt>
+                <c:pt idx="363">
+                  <c:v>2022-06-16 18:00</c:v>
+                </c:pt>
+                <c:pt idx="364">
+                  <c:v>2022-06-16 19:00</c:v>
+                </c:pt>
+                <c:pt idx="365">
+                  <c:v>2022-06-16 20:00</c:v>
+                </c:pt>
+                <c:pt idx="366">
+                  <c:v>2022-06-16 21:00</c:v>
+                </c:pt>
+                <c:pt idx="367">
+                  <c:v>2022-06-16 22:00</c:v>
+                </c:pt>
+                <c:pt idx="368">
+                  <c:v>2022-06-16 23:00</c:v>
+                </c:pt>
+                <c:pt idx="369">
+                  <c:v>2022-06-17 00:00</c:v>
+                </c:pt>
+                <c:pt idx="370">
+                  <c:v>2022-06-17 01:00</c:v>
+                </c:pt>
+                <c:pt idx="371">
+                  <c:v>2022-06-17 02:00</c:v>
+                </c:pt>
+                <c:pt idx="372">
+                  <c:v>2022-06-17 03:00</c:v>
+                </c:pt>
+                <c:pt idx="373">
+                  <c:v>2022-06-17 04:00</c:v>
+                </c:pt>
+                <c:pt idx="374">
+                  <c:v>2022-06-17 05:00</c:v>
+                </c:pt>
+                <c:pt idx="375">
+                  <c:v>2022-06-17 06:00</c:v>
+                </c:pt>
+                <c:pt idx="376">
+                  <c:v>2022-06-17 07:00</c:v>
+                </c:pt>
+                <c:pt idx="377">
+                  <c:v>2022-06-17 08:00</c:v>
+                </c:pt>
+                <c:pt idx="378">
+                  <c:v>2022-06-17 09:00</c:v>
+                </c:pt>
+                <c:pt idx="379">
+                  <c:v>2022-06-17 10:00</c:v>
+                </c:pt>
+                <c:pt idx="380">
+                  <c:v>2022-06-17 11:00</c:v>
+                </c:pt>
+                <c:pt idx="381">
+                  <c:v>2022-06-17 12:00</c:v>
+                </c:pt>
+                <c:pt idx="382">
+                  <c:v>2022-06-17 13:00</c:v>
+                </c:pt>
+                <c:pt idx="383">
+                  <c:v>2022-06-17 14:00</c:v>
+                </c:pt>
+                <c:pt idx="384">
+                  <c:v>2022-06-17 15:00</c:v>
+                </c:pt>
+                <c:pt idx="385">
+                  <c:v>2022-06-17 16:00</c:v>
+                </c:pt>
+                <c:pt idx="386">
+                  <c:v>2022-06-17 17:00</c:v>
+                </c:pt>
+                <c:pt idx="387">
+                  <c:v>2022-06-17 18:00</c:v>
+                </c:pt>
+                <c:pt idx="388">
+                  <c:v>2022-06-17 19:00</c:v>
+                </c:pt>
+                <c:pt idx="389">
+                  <c:v>2022-06-17 20:00</c:v>
+                </c:pt>
+                <c:pt idx="390">
+                  <c:v>2022-06-17 21:00</c:v>
+                </c:pt>
+                <c:pt idx="391">
+                  <c:v>2022-06-17 22:00</c:v>
+                </c:pt>
+                <c:pt idx="392">
+                  <c:v>2022-06-17 23:00</c:v>
+                </c:pt>
+                <c:pt idx="393">
+                  <c:v>2022-06-18 00:00</c:v>
+                </c:pt>
+                <c:pt idx="394">
+                  <c:v>2022-06-18 01:00</c:v>
+                </c:pt>
+                <c:pt idx="395">
+                  <c:v>2022-06-18 02:00</c:v>
+                </c:pt>
+                <c:pt idx="396">
+                  <c:v>2022-06-18 03:00</c:v>
+                </c:pt>
+                <c:pt idx="397">
+                  <c:v>2022-06-18 04:00</c:v>
+                </c:pt>
+                <c:pt idx="398">
+                  <c:v>2022-06-18 05:00</c:v>
+                </c:pt>
+                <c:pt idx="399">
+                  <c:v>2022-06-18 06:00</c:v>
+                </c:pt>
+                <c:pt idx="400">
+                  <c:v>2022-06-18 07:00</c:v>
+                </c:pt>
+                <c:pt idx="401">
+                  <c:v>2022-06-18 08:00</c:v>
+                </c:pt>
+                <c:pt idx="402">
+                  <c:v>2022-06-18 09:00</c:v>
+                </c:pt>
+                <c:pt idx="403">
+                  <c:v>2022-06-18 10:00</c:v>
+                </c:pt>
+                <c:pt idx="404">
+                  <c:v>2022-06-18 11:00</c:v>
+                </c:pt>
+                <c:pt idx="405">
+                  <c:v>2022-06-18 12:00</c:v>
+                </c:pt>
+                <c:pt idx="406">
+                  <c:v>2022-06-18 13:00</c:v>
+                </c:pt>
+                <c:pt idx="407">
+                  <c:v>2022-06-18 14:00</c:v>
+                </c:pt>
+                <c:pt idx="408">
+                  <c:v>2022-06-18 15:00</c:v>
+                </c:pt>
+                <c:pt idx="409">
+                  <c:v>2022-06-18 16:00</c:v>
+                </c:pt>
+                <c:pt idx="410">
+                  <c:v>2022-06-18 17:00</c:v>
+                </c:pt>
+                <c:pt idx="411">
+                  <c:v>2022-06-18 18:00</c:v>
+                </c:pt>
+                <c:pt idx="412">
+                  <c:v>2022-06-18 19:00</c:v>
+                </c:pt>
+                <c:pt idx="413">
+                  <c:v>2022-06-18 20:00</c:v>
+                </c:pt>
+                <c:pt idx="414">
+                  <c:v>2022-06-18 21:00</c:v>
+                </c:pt>
+                <c:pt idx="415">
+                  <c:v>2022-06-18 22:00</c:v>
+                </c:pt>
+                <c:pt idx="416">
+                  <c:v>2022-06-18 23:00</c:v>
+                </c:pt>
+                <c:pt idx="417">
+                  <c:v>2022-06-19 00:00</c:v>
+                </c:pt>
+                <c:pt idx="418">
+                  <c:v>2022-06-19 01:00</c:v>
+                </c:pt>
+                <c:pt idx="419">
+                  <c:v>2022-06-19 02:00</c:v>
+                </c:pt>
+                <c:pt idx="420">
+                  <c:v>2022-06-19 03:00</c:v>
+                </c:pt>
+                <c:pt idx="421">
+                  <c:v>2022-06-19 04:00</c:v>
+                </c:pt>
+                <c:pt idx="422">
+                  <c:v>2022-06-19 05:00</c:v>
+                </c:pt>
+                <c:pt idx="423">
+                  <c:v>2022-06-19 06:00</c:v>
+                </c:pt>
+                <c:pt idx="424">
+                  <c:v>2022-06-19 07:00</c:v>
+                </c:pt>
+                <c:pt idx="425">
+                  <c:v>2022-06-19 08:00</c:v>
+                </c:pt>
+                <c:pt idx="426">
+                  <c:v>2022-06-19 09:00</c:v>
+                </c:pt>
+                <c:pt idx="427">
+                  <c:v>2022-06-19 10:00</c:v>
+                </c:pt>
+                <c:pt idx="428">
+                  <c:v>2022-06-19 11:00</c:v>
+                </c:pt>
+                <c:pt idx="429">
+                  <c:v>2022-06-19 12:00</c:v>
+                </c:pt>
+                <c:pt idx="430">
+                  <c:v>2022-06-19 13:00</c:v>
+                </c:pt>
+                <c:pt idx="431">
+                  <c:v>2022-06-19 14:00</c:v>
+                </c:pt>
+                <c:pt idx="432">
+                  <c:v>2022-06-19 15:00</c:v>
+                </c:pt>
+                <c:pt idx="433">
+                  <c:v>2022-06-19 16:00</c:v>
+                </c:pt>
+                <c:pt idx="434">
+                  <c:v>2022-06-19 17:00</c:v>
+                </c:pt>
+                <c:pt idx="435">
+                  <c:v>2022-06-19 18:00</c:v>
+                </c:pt>
+                <c:pt idx="436">
+                  <c:v>2022-06-19 19:00</c:v>
+                </c:pt>
+                <c:pt idx="437">
+                  <c:v>2022-06-19 20:00</c:v>
+                </c:pt>
+                <c:pt idx="438">
+                  <c:v>2022-06-19 21:00</c:v>
+                </c:pt>
+                <c:pt idx="439">
+                  <c:v>2022-06-19 22:00</c:v>
+                </c:pt>
+                <c:pt idx="440">
+                  <c:v>2022-06-19 23:00</c:v>
+                </c:pt>
+                <c:pt idx="441">
+                  <c:v>2022-06-20 00:00</c:v>
+                </c:pt>
+                <c:pt idx="442">
+                  <c:v>2022-06-20 01:00</c:v>
+                </c:pt>
+                <c:pt idx="443">
+                  <c:v>2022-06-20 02:00</c:v>
+                </c:pt>
+                <c:pt idx="444">
+                  <c:v>2022-06-20 03:00</c:v>
+                </c:pt>
+                <c:pt idx="445">
+                  <c:v>2022-06-20 04:00</c:v>
+                </c:pt>
+                <c:pt idx="446">
+                  <c:v>2022-06-20 05:00</c:v>
+                </c:pt>
+                <c:pt idx="447">
+                  <c:v>2022-06-20 06:00</c:v>
+                </c:pt>
+                <c:pt idx="448">
+                  <c:v>2022-06-20 07:00</c:v>
+                </c:pt>
+                <c:pt idx="449">
+                  <c:v>2022-06-20 08:00</c:v>
+                </c:pt>
+                <c:pt idx="450">
+                  <c:v>2022-06-20 09:00</c:v>
+                </c:pt>
+                <c:pt idx="451">
+                  <c:v>2022-06-20 10:00</c:v>
+                </c:pt>
+                <c:pt idx="452">
+                  <c:v>2022-06-20 11:00</c:v>
+                </c:pt>
+                <c:pt idx="453">
+                  <c:v>2022-06-20 12:00</c:v>
+                </c:pt>
+                <c:pt idx="454">
+                  <c:v>2022-06-20 13:00</c:v>
+                </c:pt>
+                <c:pt idx="455">
+                  <c:v>2022-06-20 14:00</c:v>
+                </c:pt>
+                <c:pt idx="456">
+                  <c:v>2022-06-20 15:00</c:v>
+                </c:pt>
+                <c:pt idx="457">
+                  <c:v>2022-06-20 16:00</c:v>
+                </c:pt>
+                <c:pt idx="458">
+                  <c:v>2022-06-20 17:00</c:v>
+                </c:pt>
+                <c:pt idx="459">
+                  <c:v>2022-06-20 18:00</c:v>
+                </c:pt>
+                <c:pt idx="460">
+                  <c:v>2022-06-20 19:00</c:v>
+                </c:pt>
+                <c:pt idx="461">
+                  <c:v>2022-06-20 20:00</c:v>
+                </c:pt>
+                <c:pt idx="462">
+                  <c:v>2022-06-20 21:00</c:v>
+                </c:pt>
+                <c:pt idx="463">
+                  <c:v>2022-06-20 22:00</c:v>
+                </c:pt>
+                <c:pt idx="464">
+                  <c:v>2022-06-20 23:00</c:v>
+                </c:pt>
+                <c:pt idx="465">
+                  <c:v>2022-06-21 00:00</c:v>
+                </c:pt>
+                <c:pt idx="466">
+                  <c:v>2022-06-21 01:00</c:v>
+                </c:pt>
+                <c:pt idx="467">
+                  <c:v>2022-06-21 02:00</c:v>
+                </c:pt>
+                <c:pt idx="468">
+                  <c:v>2022-06-21 03:00</c:v>
+                </c:pt>
+                <c:pt idx="469">
+                  <c:v>2022-06-21 04:00</c:v>
+                </c:pt>
+                <c:pt idx="470">
+                  <c:v>2022-06-21 05:00</c:v>
+                </c:pt>
+                <c:pt idx="471">
+                  <c:v>2022-06-21 06:00</c:v>
+                </c:pt>
+                <c:pt idx="472">
+                  <c:v>2022-06-21 07:00</c:v>
+                </c:pt>
+                <c:pt idx="473">
+                  <c:v>2022-06-21 08:00</c:v>
+                </c:pt>
+                <c:pt idx="474">
+                  <c:v>2022-06-21 09:00</c:v>
+                </c:pt>
+                <c:pt idx="475">
+                  <c:v>2022-06-21 10:00</c:v>
+                </c:pt>
+                <c:pt idx="476">
+                  <c:v>2022-06-21 11:00</c:v>
+                </c:pt>
+                <c:pt idx="477">
+                  <c:v>2022-06-21 12:00</c:v>
+                </c:pt>
+                <c:pt idx="478">
+                  <c:v>2022-06-21 13:00</c:v>
+                </c:pt>
+                <c:pt idx="479">
+                  <c:v>2022-06-21 14:00</c:v>
+                </c:pt>
+                <c:pt idx="480">
+                  <c:v>2022-06-21 15:00</c:v>
+                </c:pt>
+                <c:pt idx="481">
+                  <c:v>2022-06-21 16:00</c:v>
+                </c:pt>
+                <c:pt idx="482">
+                  <c:v>2022-06-21 17:00</c:v>
+                </c:pt>
+                <c:pt idx="483">
+                  <c:v>2022-06-21 18:00</c:v>
+                </c:pt>
+                <c:pt idx="484">
+                  <c:v>2022-06-21 19:00</c:v>
+                </c:pt>
+                <c:pt idx="485">
+                  <c:v>2022-06-21 20:00</c:v>
+                </c:pt>
+                <c:pt idx="486">
+                  <c:v>2022-06-21 21:00</c:v>
+                </c:pt>
+                <c:pt idx="487">
+                  <c:v>2022-06-21 22:00</c:v>
+                </c:pt>
+                <c:pt idx="488">
+                  <c:v>2022-06-21 23:00</c:v>
+                </c:pt>
+                <c:pt idx="489">
+                  <c:v>2022-06-22 00:00</c:v>
+                </c:pt>
+                <c:pt idx="490">
+                  <c:v>2022-06-22 01:00</c:v>
+                </c:pt>
+                <c:pt idx="491">
+                  <c:v>2022-06-22 02:00</c:v>
+                </c:pt>
+                <c:pt idx="492">
+                  <c:v>2022-06-22 03:00</c:v>
+                </c:pt>
+                <c:pt idx="493">
+                  <c:v>2022-06-22 04:00</c:v>
+                </c:pt>
+                <c:pt idx="494">
+                  <c:v>2022-06-22 05:00</c:v>
+                </c:pt>
+                <c:pt idx="495">
+                  <c:v>2022-06-22 06:00</c:v>
+                </c:pt>
+                <c:pt idx="496">
+                  <c:v>2022-06-22 07:00</c:v>
+                </c:pt>
+                <c:pt idx="497">
+                  <c:v>2022-06-22 08:00</c:v>
+                </c:pt>
+                <c:pt idx="498">
+                  <c:v>2022-06-22 09:00</c:v>
+                </c:pt>
+                <c:pt idx="499">
+                  <c:v>2022-06-22 10:00</c:v>
+                </c:pt>
+                <c:pt idx="500">
+                  <c:v>2022-06-22 11:00</c:v>
+                </c:pt>
+                <c:pt idx="501">
+                  <c:v>2022-06-22 12:00</c:v>
+                </c:pt>
+                <c:pt idx="502">
+                  <c:v>2022-06-22 13:00</c:v>
+                </c:pt>
+                <c:pt idx="503">
+                  <c:v>2022-06-22 14:00</c:v>
+                </c:pt>
+                <c:pt idx="504">
+                  <c:v>2022-06-22 15:00</c:v>
+                </c:pt>
+                <c:pt idx="505">
+                  <c:v>2022-06-22 16:00</c:v>
+                </c:pt>
+                <c:pt idx="506">
+                  <c:v>2022-06-22 17:00</c:v>
+                </c:pt>
+                <c:pt idx="507">
+                  <c:v>2022-06-22 18:00</c:v>
+                </c:pt>
+                <c:pt idx="508">
+                  <c:v>2022-06-22 19:00</c:v>
+                </c:pt>
+                <c:pt idx="509">
+                  <c:v>2022-06-22 20:00</c:v>
+                </c:pt>
+                <c:pt idx="510">
+                  <c:v>2022-06-22 21:00</c:v>
+                </c:pt>
+                <c:pt idx="511">
+                  <c:v>2022-06-22 22:00</c:v>
+                </c:pt>
+                <c:pt idx="512">
+                  <c:v>2022-06-22 23:00</c:v>
+                </c:pt>
+                <c:pt idx="513">
+                  <c:v>2022-06-23 00:00</c:v>
+                </c:pt>
+                <c:pt idx="514">
+                  <c:v>2022-06-23 01:00</c:v>
+                </c:pt>
+                <c:pt idx="515">
+                  <c:v>2022-06-23 02:00</c:v>
+                </c:pt>
+                <c:pt idx="516">
+                  <c:v>2022-06-23 03:00</c:v>
+                </c:pt>
+                <c:pt idx="517">
+                  <c:v>2022-06-23 04:00</c:v>
+                </c:pt>
+                <c:pt idx="518">
+                  <c:v>2022-06-23 05:00</c:v>
+                </c:pt>
+                <c:pt idx="519">
+                  <c:v>2022-06-23 06:00</c:v>
+                </c:pt>
+                <c:pt idx="520">
+                  <c:v>2022-06-23 07:00</c:v>
+                </c:pt>
+                <c:pt idx="521">
+                  <c:v>2022-06-23 08:00</c:v>
+                </c:pt>
+                <c:pt idx="522">
+                  <c:v>2022-06-23 09:00</c:v>
+                </c:pt>
+                <c:pt idx="523">
+                  <c:v>2022-06-23 10:00</c:v>
+                </c:pt>
+                <c:pt idx="524">
+                  <c:v>2022-06-23 11:00</c:v>
+                </c:pt>
+                <c:pt idx="525">
+                  <c:v>2022-06-23 12:00</c:v>
+                </c:pt>
+                <c:pt idx="526">
+                  <c:v>2022-06-23 13:00</c:v>
+                </c:pt>
+                <c:pt idx="527">
+                  <c:v>2022-06-23 14:00</c:v>
+                </c:pt>
+                <c:pt idx="528">
+                  <c:v>2022-06-23 15:00</c:v>
+                </c:pt>
+                <c:pt idx="529">
+                  <c:v>2022-06-23 16:00</c:v>
+                </c:pt>
+                <c:pt idx="530">
+                  <c:v>2022-06-23 17:00</c:v>
+                </c:pt>
+                <c:pt idx="531">
+                  <c:v>2022-06-23 18:00</c:v>
+                </c:pt>
+                <c:pt idx="532">
+                  <c:v>2022-06-23 19:00</c:v>
+                </c:pt>
+                <c:pt idx="533">
+                  <c:v>2022-06-23 20:00</c:v>
+                </c:pt>
+                <c:pt idx="534">
+                  <c:v>2022-06-23 21:00</c:v>
+                </c:pt>
+                <c:pt idx="535">
+                  <c:v>2022-06-23 22:00</c:v>
+                </c:pt>
+                <c:pt idx="536">
+                  <c:v>2022-06-23 23:00</c:v>
+                </c:pt>
+                <c:pt idx="537">
+                  <c:v>2022-06-24 00:00</c:v>
+                </c:pt>
+                <c:pt idx="538">
+                  <c:v>2022-06-24 01:00</c:v>
+                </c:pt>
+                <c:pt idx="539">
+                  <c:v>2022-06-24 02:00</c:v>
+                </c:pt>
+                <c:pt idx="540">
+                  <c:v>2022-06-24 03:00</c:v>
+                </c:pt>
+                <c:pt idx="541">
+                  <c:v>2022-06-24 04:00</c:v>
+                </c:pt>
+                <c:pt idx="542">
+                  <c:v>2022-06-24 05:00</c:v>
+                </c:pt>
+                <c:pt idx="543">
+                  <c:v>2022-06-24 06:00</c:v>
+                </c:pt>
+                <c:pt idx="544">
+                  <c:v>2022-06-24 07:00</c:v>
+                </c:pt>
+                <c:pt idx="545">
+                  <c:v>2022-06-24 08:00</c:v>
+                </c:pt>
+                <c:pt idx="546">
+                  <c:v>2022-06-24 09:00</c:v>
+                </c:pt>
+                <c:pt idx="547">
+                  <c:v>2022-06-24 10:00</c:v>
+                </c:pt>
+                <c:pt idx="548">
+                  <c:v>2022-06-24 11:00</c:v>
+                </c:pt>
+                <c:pt idx="549">
+                  <c:v>2022-06-24 12:00</c:v>
+                </c:pt>
+                <c:pt idx="550">
+                  <c:v>2022-06-24 13:00</c:v>
+                </c:pt>
+                <c:pt idx="551">
+                  <c:v>2022-06-24 14:00</c:v>
+                </c:pt>
+                <c:pt idx="552">
+                  <c:v>2022-06-24 15:00</c:v>
+                </c:pt>
+                <c:pt idx="553">
+                  <c:v>2022-06-24 16:00</c:v>
+                </c:pt>
+                <c:pt idx="554">
+                  <c:v>2022-06-24 17:00</c:v>
+                </c:pt>
+                <c:pt idx="555">
+                  <c:v>2022-06-24 18:00</c:v>
+                </c:pt>
+                <c:pt idx="556">
+                  <c:v>2022-06-24 19:00</c:v>
+                </c:pt>
+                <c:pt idx="557">
+                  <c:v>2022-06-24 20:00</c:v>
+                </c:pt>
+                <c:pt idx="558">
+                  <c:v>2022-06-24 21:00</c:v>
+                </c:pt>
+                <c:pt idx="559">
+                  <c:v>2022-06-24 22:00</c:v>
+                </c:pt>
+                <c:pt idx="560">
+                  <c:v>2022-06-24 23:00</c:v>
+                </c:pt>
+                <c:pt idx="561">
+                  <c:v>2022-06-25 00:00</c:v>
+                </c:pt>
+                <c:pt idx="562">
+                  <c:v>2022-06-25 01:00</c:v>
+                </c:pt>
+                <c:pt idx="563">
+                  <c:v>2022-06-25 02:00</c:v>
+                </c:pt>
+                <c:pt idx="564">
+                  <c:v>2022-06-25 03:00</c:v>
+                </c:pt>
+                <c:pt idx="565">
+                  <c:v>2022-06-25 04:00</c:v>
+                </c:pt>
+                <c:pt idx="566">
+                  <c:v>2022-06-25 05:00</c:v>
+                </c:pt>
+                <c:pt idx="567">
+                  <c:v>2022-06-25 06:00</c:v>
+                </c:pt>
+                <c:pt idx="568">
+                  <c:v>2022-06-25 07:00</c:v>
+                </c:pt>
+                <c:pt idx="569">
+                  <c:v>2022-06-25 08:00</c:v>
+                </c:pt>
+                <c:pt idx="570">
+                  <c:v>2022-06-25 09:00</c:v>
+                </c:pt>
+                <c:pt idx="571">
+                  <c:v>2022-06-25 10:00</c:v>
+                </c:pt>
+                <c:pt idx="572">
+                  <c:v>2022-06-25 11:00</c:v>
+                </c:pt>
+                <c:pt idx="573">
+                  <c:v>2022-06-25 12:00</c:v>
+                </c:pt>
+                <c:pt idx="574">
+                  <c:v>2022-06-25 13:00</c:v>
+                </c:pt>
+                <c:pt idx="575">
+                  <c:v>2022-06-25 14:00</c:v>
+                </c:pt>
+                <c:pt idx="576">
+                  <c:v>2022-06-25 15:00</c:v>
+                </c:pt>
+                <c:pt idx="577">
+                  <c:v>2022-06-25 16:00</c:v>
+                </c:pt>
+                <c:pt idx="578">
+                  <c:v>2022-06-25 17:00</c:v>
+                </c:pt>
+                <c:pt idx="579">
+                  <c:v>2022-06-25 18:00</c:v>
+                </c:pt>
+                <c:pt idx="580">
+                  <c:v>2022-06-25 19:00</c:v>
+                </c:pt>
+                <c:pt idx="581">
+                  <c:v>2022-06-25 20:00</c:v>
+                </c:pt>
+                <c:pt idx="582">
+                  <c:v>2022-06-25 21:00</c:v>
+                </c:pt>
+                <c:pt idx="583">
+                  <c:v>2022-06-25 22:00</c:v>
+                </c:pt>
+                <c:pt idx="584">
+                  <c:v>2022-06-25 23:00</c:v>
+                </c:pt>
+                <c:pt idx="585">
+                  <c:v>2022-06-26 00:00</c:v>
+                </c:pt>
+                <c:pt idx="586">
+                  <c:v>2022-06-26 01:00</c:v>
+                </c:pt>
+                <c:pt idx="587">
+                  <c:v>2022-06-26 02:00</c:v>
+                </c:pt>
+                <c:pt idx="588">
+                  <c:v>2022-06-26 03:00</c:v>
+                </c:pt>
+                <c:pt idx="589">
+                  <c:v>2022-06-26 04:00</c:v>
+                </c:pt>
+                <c:pt idx="590">
+                  <c:v>2022-06-26 05:00</c:v>
+                </c:pt>
+                <c:pt idx="591">
+                  <c:v>2022-06-26 06:00</c:v>
+                </c:pt>
+                <c:pt idx="592">
+                  <c:v>2022-06-26 07:00</c:v>
+                </c:pt>
+                <c:pt idx="593">
+                  <c:v>2022-06-26 08:00</c:v>
+                </c:pt>
+                <c:pt idx="594">
+                  <c:v>2022-06-26 09:00</c:v>
+                </c:pt>
+                <c:pt idx="595">
+                  <c:v>2022-06-26 10:00</c:v>
+                </c:pt>
+                <c:pt idx="596">
+                  <c:v>2022-06-26 11:00</c:v>
+                </c:pt>
+                <c:pt idx="597">
+                  <c:v>2022-06-26 12:00</c:v>
+                </c:pt>
+                <c:pt idx="598">
+                  <c:v>2022-06-26 13:00</c:v>
+                </c:pt>
+                <c:pt idx="599">
+                  <c:v>2022-06-26 14:00</c:v>
+                </c:pt>
+                <c:pt idx="600">
+                  <c:v>2022-06-26 15:00</c:v>
+                </c:pt>
+                <c:pt idx="601">
+                  <c:v>2022-06-26 16:00</c:v>
+                </c:pt>
+                <c:pt idx="602">
+                  <c:v>2022-06-26 17:00</c:v>
+                </c:pt>
+                <c:pt idx="603">
+                  <c:v>2022-06-26 18:00</c:v>
+                </c:pt>
+                <c:pt idx="604">
+                  <c:v>2022-06-26 19:00</c:v>
+                </c:pt>
+                <c:pt idx="605">
+                  <c:v>2022-06-26 20:00</c:v>
+                </c:pt>
+                <c:pt idx="606">
+                  <c:v>2022-06-26 21:00</c:v>
+                </c:pt>
+                <c:pt idx="607">
+                  <c:v>2022-06-26 22:00</c:v>
+                </c:pt>
+                <c:pt idx="608">
+                  <c:v>2022-06-26 23:00</c:v>
+                </c:pt>
+                <c:pt idx="609">
+                  <c:v>2022-06-27 00:00</c:v>
+                </c:pt>
+                <c:pt idx="610">
+                  <c:v>2022-06-27 01:00</c:v>
+                </c:pt>
+                <c:pt idx="611">
+                  <c:v>2022-06-27 02:00</c:v>
+                </c:pt>
+                <c:pt idx="612">
+                  <c:v>2022-06-27 03:00</c:v>
+                </c:pt>
+                <c:pt idx="613">
+                  <c:v>2022-06-27 04:00</c:v>
+                </c:pt>
+                <c:pt idx="614">
+                  <c:v>2022-06-27 05:00</c:v>
+                </c:pt>
+                <c:pt idx="615">
+                  <c:v>2022-06-27 06:00</c:v>
+                </c:pt>
+                <c:pt idx="616">
+                  <c:v>2022-06-27 07:00</c:v>
+                </c:pt>
+                <c:pt idx="617">
+                  <c:v>2022-06-27 08:00</c:v>
+                </c:pt>
+                <c:pt idx="618">
+                  <c:v>2022-06-27 09:00</c:v>
+                </c:pt>
+                <c:pt idx="619">
+                  <c:v>2022-06-27 10:00</c:v>
+                </c:pt>
+                <c:pt idx="620">
+                  <c:v>2022-06-27 11:00</c:v>
+                </c:pt>
+                <c:pt idx="621">
+                  <c:v>2022-06-27 12:00</c:v>
+                </c:pt>
+                <c:pt idx="622">
+                  <c:v>2022-06-27 13:00</c:v>
+                </c:pt>
+                <c:pt idx="623">
+                  <c:v>2022-06-27 14:00</c:v>
+                </c:pt>
+                <c:pt idx="624">
+                  <c:v>2022-06-27 15:00</c:v>
+                </c:pt>
+                <c:pt idx="625">
+                  <c:v>2022-06-27 16:00</c:v>
+                </c:pt>
+                <c:pt idx="626">
+                  <c:v>2022-06-27 17:00</c:v>
+                </c:pt>
+                <c:pt idx="627">
+                  <c:v>2022-06-27 18:00</c:v>
+                </c:pt>
+                <c:pt idx="628">
+                  <c:v>2022-06-27 19:00</c:v>
+                </c:pt>
+                <c:pt idx="629">
+                  <c:v>2022-06-27 20:00</c:v>
+                </c:pt>
+                <c:pt idx="630">
+                  <c:v>2022-06-27 21:00</c:v>
+                </c:pt>
+                <c:pt idx="631">
+                  <c:v>2022-06-27 22:00</c:v>
+                </c:pt>
+                <c:pt idx="632">
+                  <c:v>2022-06-27 23:00</c:v>
+                </c:pt>
+                <c:pt idx="633">
+                  <c:v>2022-06-28 00:00</c:v>
+                </c:pt>
+                <c:pt idx="634">
+                  <c:v>2022-06-28 01:00</c:v>
+                </c:pt>
+                <c:pt idx="635">
+                  <c:v>2022-06-28 02:00</c:v>
+                </c:pt>
+                <c:pt idx="636">
+                  <c:v>2022-06-28 03:00</c:v>
+                </c:pt>
+                <c:pt idx="637">
+                  <c:v>2022-06-28 04:00</c:v>
+                </c:pt>
+                <c:pt idx="638">
+                  <c:v>2022-06-28 05:00</c:v>
+                </c:pt>
+                <c:pt idx="639">
+                  <c:v>2022-06-28 06:00</c:v>
+                </c:pt>
+                <c:pt idx="640">
+                  <c:v>2022-06-28 07:00</c:v>
+                </c:pt>
+                <c:pt idx="641">
+                  <c:v>2022-06-28 08:00</c:v>
+                </c:pt>
+                <c:pt idx="642">
+                  <c:v>2022-06-28 09:00</c:v>
+                </c:pt>
+                <c:pt idx="643">
+                  <c:v>2022-06-28 10:00</c:v>
+                </c:pt>
+                <c:pt idx="644">
+                  <c:v>2022-06-28 11:00</c:v>
+                </c:pt>
+                <c:pt idx="645">
+                  <c:v>2022-06-28 12:00</c:v>
+                </c:pt>
+                <c:pt idx="646">
+                  <c:v>2022-06-28 13:00</c:v>
+                </c:pt>
+                <c:pt idx="647">
+                  <c:v>2022-06-28 14:00</c:v>
+                </c:pt>
+                <c:pt idx="648">
+                  <c:v>2022-06-28 15:00</c:v>
+                </c:pt>
+                <c:pt idx="649">
+                  <c:v>2022-06-28 16:00</c:v>
+                </c:pt>
+                <c:pt idx="650">
+                  <c:v>2022-06-28 17:00</c:v>
+                </c:pt>
+                <c:pt idx="651">
+                  <c:v>2022-06-28 18:00</c:v>
+                </c:pt>
+                <c:pt idx="652">
+                  <c:v>2022-06-28 19:00</c:v>
+                </c:pt>
+                <c:pt idx="653">
+                  <c:v>2022-06-28 20:00</c:v>
+                </c:pt>
+                <c:pt idx="654">
+                  <c:v>2022-06-28 21:00</c:v>
+                </c:pt>
+                <c:pt idx="655">
+                  <c:v>2022-06-28 22:00</c:v>
+                </c:pt>
+                <c:pt idx="656">
+                  <c:v>2022-06-28 23:00</c:v>
+                </c:pt>
+                <c:pt idx="657">
+                  <c:v>2022-06-29 00:00</c:v>
+                </c:pt>
+                <c:pt idx="658">
+                  <c:v>2022-06-29 01:00</c:v>
+                </c:pt>
+                <c:pt idx="659">
+                  <c:v>2022-06-29 02:00</c:v>
+                </c:pt>
+                <c:pt idx="660">
+                  <c:v>2022-06-29 03:00</c:v>
+                </c:pt>
+                <c:pt idx="661">
+                  <c:v>2022-06-29 04:00</c:v>
+                </c:pt>
+                <c:pt idx="662">
+                  <c:v>2022-06-29 05:00</c:v>
+                </c:pt>
+                <c:pt idx="663">
+                  <c:v>2022-06-29 06:00</c:v>
+                </c:pt>
+                <c:pt idx="664">
+                  <c:v>2022-06-29 07:00</c:v>
+                </c:pt>
+                <c:pt idx="665">
+                  <c:v>2022-06-29 08:00</c:v>
+                </c:pt>
+                <c:pt idx="666">
+                  <c:v>2022-06-29 09:00</c:v>
+                </c:pt>
+                <c:pt idx="667">
+                  <c:v>2022-06-29 10:00</c:v>
+                </c:pt>
+                <c:pt idx="668">
+                  <c:v>2022-06-29 11:00</c:v>
+                </c:pt>
+                <c:pt idx="669">
+                  <c:v>2022-06-29 12:00</c:v>
+                </c:pt>
+                <c:pt idx="670">
+                  <c:v>2022-06-29 13:00</c:v>
+                </c:pt>
+                <c:pt idx="671">
+                  <c:v>2022-06-29 14:00</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$17:$B$688</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="672"/>
+                <c:pt idx="0">
+                  <c:v>1388.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1425.09</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1408.68</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1221.58</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1088.53</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>787.11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>446.97</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>413.09</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>383.04</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>343.17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>312.18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>225.24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>217.74</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>214.06</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>215.91</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>219.24</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>671.53</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1211.3599999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1270.8900000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1458.42</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1469.63</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1488.31</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1479.85</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1471.28</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1520.78</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1512.43</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1460.14</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1406.1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1241.18</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1055.6400000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1045.83</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>912.87</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>498.29</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>359.08</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>335.56</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>235.84</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>237.28</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>238.05</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>232.42</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>243.79</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>559.29</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1231.56</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1323.43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1370.06</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1378.8</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1391.69</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1382.49</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1394.13</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1401.75</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1397.84</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1415.64</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1386.12</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1253.1099999999999</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1143.8699999999999</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1024.32</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1020.92</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>519.28</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>387.33</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>352.18</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>256.62</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>258.36</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>257.19</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>251.89</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>292.41000000000003</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>562.27</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1139.07</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>940.72</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>955.74</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>964.15</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>981.81</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>980.68</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>956.47</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>918.29</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>893.12</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>859.48</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>820.17</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>375.07</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>63.7</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>53.12</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>45.34</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1355.89</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>272</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>202.51</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>190.44</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>195.32</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>198.19</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>196.48</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>239.52</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>609.96</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1053.53</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1081.68</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1074.8399999999999</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1088.02</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1100.1300000000001</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1062.18</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1094.3699999999999</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1097.7</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1091.48</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1006.3</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>926.55</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>428.87</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>418</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>916.25</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>783.8</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>710.07</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>661.2</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>405.4</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>211.05</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>212.21</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>215.31</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>578.48</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>1163.6600000000001</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1258.48</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1460.96</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>1511.35</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1490.95</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1514.66</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1509.38</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>1542.77</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>1522.91</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>1512.53</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>1400.08</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>1199.26</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>1178.01</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>1110.5899999999999</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>989.24</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>857.87</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>847.85</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>401.15</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>252.73</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>243.1</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>241.54</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>232.8</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>247.5</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>747.29</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>1238.01</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>1496.03</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>1517.77</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>1518.12</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>1523.13</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>1498.98</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>1539.09</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>1561.41</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>1257.9000000000001</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>1441.52</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>1386.91</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>1303.4000000000001</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>1178.96</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>1119.83</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>1048.97</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>918.41</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>859.11</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>819.21</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>761.38</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>550.13</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>254.6</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>254.39</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>295.58999999999997</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>1035.71</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>1181.22</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>1454.72</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>1447.56</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>1451.58</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>1417.86</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>1401.15</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>1395.93</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>1428.81</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>1414.23</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>1396.33</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>1180.6199999999999</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>1046.6600000000001</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>970.25</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>932.99</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>904.78</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>517.26</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>372.23</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>333.57</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>248.1</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>241.24</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>232.74</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>249.9</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>283.10000000000002</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>1088.7</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>1029.53</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>1295.81</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>1257.21</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>1225.8399999999999</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>1228.1400000000001</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>1183.57</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>1257.5</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>1341.97</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>1423.49</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>1263.8499999999999</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>1092.3699999999999</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>996.48</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>875.05</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>635.41999999999996</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>420.95</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>401.71</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>347.09</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>313.98</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>216.93</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>211.64</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>205.37</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>208.5</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>227.08</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>952.2</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>1045.01</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>1254.54</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>1318.2</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>1310.7</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>1351.97</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>1321.93</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>1284.3399999999999</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>1302.3499999999999</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>1290.05</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>1153.6099999999999</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>1026.0899999999999</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>926.41</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>875.91</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>888.29</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>887</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>685.62</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>335.99</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>308.64999999999998</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>220.6</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>218.11</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>219.6</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>220.53</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>280.39</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>963.59</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>880.04</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>1094.3800000000001</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>1111.51</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>1130.53</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>1120.1300000000001</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>1050.43</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>1088.54</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>1103.46</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>1061.27</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>1054.6300000000001</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>975.94</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>977.8</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>937.77</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>482.02</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>396.94</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>394.32</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>333.81</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>295.52999999999997</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>207.29</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>212.81</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>201.16</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>197.35</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>218.59</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>864.23</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>873.97</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>971.56</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>1088.79</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>1115.43</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>1227.72</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>1203.56</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>1317.43</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>1171.54</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>1365.96</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>1354.5</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>1208.19</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>1139.5899999999999</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>1035.47</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>1011.9</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>975.66</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>432.24</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>341.56</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>311.8</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>218.65</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>212.03</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>214.12</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>220.86</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>1048.43</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>1203.72</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>1415.66</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>1452.82</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>1471.53</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>1508.11</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>1497.21</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>1532.64</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>1540.75</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>1556.56</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>1491.14</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>1401.14</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>1135.49</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>1053.9100000000001</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>993.25</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>943.91</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>823.25</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>500.7</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>314.08</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>226.44</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>228.25</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>215.19</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>212.18</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>309.89</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>1042.6400000000001</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>1120.03</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>1521.8</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>1569.21</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>1602.92</c:v>
+                </c:pt>
+                <c:pt idx="309">
+                  <c:v>1608.05</c:v>
+                </c:pt>
+                <c:pt idx="310">
+                  <c:v>1624.93</c:v>
+                </c:pt>
+                <c:pt idx="311">
+                  <c:v>1657.07</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>1685.59</c:v>
+                </c:pt>
+                <c:pt idx="313">
+                  <c:v>1673.37</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>1517.63</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>1416.83</c:v>
+                </c:pt>
+                <c:pt idx="316">
+                  <c:v>1403.79</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>1279.78</c:v>
+                </c:pt>
+                <c:pt idx="318">
+                  <c:v>1042.02</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>971.75</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>859.25</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>827.25</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>758.78</c:v>
+                </c:pt>
+                <c:pt idx="323">
+                  <c:v>707.3</c:v>
+                </c:pt>
+                <c:pt idx="324">
+                  <c:v>263.26</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>249.47</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>266.99</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>335.46</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>1131.8699999999999</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>1250.44</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>1573.82</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>1629.25</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>1643.28</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>1645.94</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>1665.77</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>1689.45</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>1714.63</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>1687.21</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>1498.65</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>1444.1</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>1331.94</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>1199.42</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>1070.46</c:v>
+                </c:pt>
+                <c:pt idx="343">
+                  <c:v>1014.55</c:v>
+                </c:pt>
+                <c:pt idx="344">
+                  <c:v>885.09</c:v>
+                </c:pt>
+                <c:pt idx="345">
+                  <c:v>833.17</c:v>
+                </c:pt>
+                <c:pt idx="346">
+                  <c:v>399.64</c:v>
+                </c:pt>
+                <c:pt idx="347">
+                  <c:v>291.86</c:v>
+                </c:pt>
+                <c:pt idx="348">
+                  <c:v>288.99</c:v>
+                </c:pt>
+                <c:pt idx="349">
+                  <c:v>284.52999999999997</c:v>
+                </c:pt>
+                <c:pt idx="350">
+                  <c:v>288.41000000000003</c:v>
+                </c:pt>
+                <c:pt idx="351">
+                  <c:v>317.56</c:v>
+                </c:pt>
+                <c:pt idx="352">
+                  <c:v>1264.26</c:v>
+                </c:pt>
+                <c:pt idx="353">
+                  <c:v>1297.93</c:v>
+                </c:pt>
+                <c:pt idx="354">
+                  <c:v>1426.74</c:v>
+                </c:pt>
+                <c:pt idx="355">
+                  <c:v>1514.3</c:v>
+                </c:pt>
+                <c:pt idx="356">
+                  <c:v>1821.62</c:v>
+                </c:pt>
+                <c:pt idx="357">
+                  <c:v>1806.96</c:v>
+                </c:pt>
+                <c:pt idx="358">
+                  <c:v>1801.43</c:v>
+                </c:pt>
+                <c:pt idx="359">
+                  <c:v>305.89999999999998</c:v>
+                </c:pt>
+                <c:pt idx="360">
+                  <c:v>308.89999999999998</c:v>
+                </c:pt>
+                <c:pt idx="361">
+                  <c:v>1803.77</c:v>
+                </c:pt>
+                <c:pt idx="362">
+                  <c:v>1602.85</c:v>
+                </c:pt>
+                <c:pt idx="363">
+                  <c:v>1563.15</c:v>
+                </c:pt>
+                <c:pt idx="364">
+                  <c:v>1252.27</c:v>
+                </c:pt>
+                <c:pt idx="365">
+                  <c:v>1056.48</c:v>
+                </c:pt>
+                <c:pt idx="366">
+                  <c:v>1058.3499999999999</c:v>
+                </c:pt>
+                <c:pt idx="367">
+                  <c:v>902.3</c:v>
+                </c:pt>
+                <c:pt idx="368">
+                  <c:v>459.72</c:v>
+                </c:pt>
+                <c:pt idx="369">
+                  <c:v>377.61</c:v>
+                </c:pt>
+                <c:pt idx="370">
+                  <c:v>332.94</c:v>
+                </c:pt>
+                <c:pt idx="371">
+                  <c:v>254.13</c:v>
+                </c:pt>
+                <c:pt idx="372">
+                  <c:v>247.21</c:v>
+                </c:pt>
+                <c:pt idx="373">
+                  <c:v>248.65</c:v>
+                </c:pt>
+                <c:pt idx="374">
+                  <c:v>239.94</c:v>
+                </c:pt>
+                <c:pt idx="375">
+                  <c:v>294.63</c:v>
+                </c:pt>
+                <c:pt idx="376">
+                  <c:v>1199.57</c:v>
+                </c:pt>
+                <c:pt idx="377">
+                  <c:v>1285.8599999999999</c:v>
+                </c:pt>
+                <c:pt idx="378">
+                  <c:v>1577.29</c:v>
+                </c:pt>
+                <c:pt idx="379">
+                  <c:v>1614.81</c:v>
+                </c:pt>
+                <c:pt idx="380">
+                  <c:v>1672.12</c:v>
+                </c:pt>
+                <c:pt idx="381">
+                  <c:v>1641.02</c:v>
+                </c:pt>
+                <c:pt idx="382">
+                  <c:v>1628.68</c:v>
+                </c:pt>
+                <c:pt idx="383">
+                  <c:v>1673.08</c:v>
+                </c:pt>
+                <c:pt idx="384">
+                  <c:v>1644.14</c:v>
+                </c:pt>
+                <c:pt idx="385">
+                  <c:v>1646.61</c:v>
+                </c:pt>
+                <c:pt idx="386">
+                  <c:v>1449.18</c:v>
+                </c:pt>
+                <c:pt idx="387">
+                  <c:v>1315.19</c:v>
+                </c:pt>
+                <c:pt idx="388">
+                  <c:v>1207.9000000000001</c:v>
+                </c:pt>
+                <c:pt idx="389">
+                  <c:v>1118.6600000000001</c:v>
+                </c:pt>
+                <c:pt idx="390">
+                  <c:v>1044.27</c:v>
+                </c:pt>
+                <c:pt idx="391">
+                  <c:v>971.17</c:v>
+                </c:pt>
+                <c:pt idx="392">
+                  <c:v>919.6</c:v>
+                </c:pt>
+                <c:pt idx="393">
+                  <c:v>517.25</c:v>
+                </c:pt>
+                <c:pt idx="394">
+                  <c:v>346.63</c:v>
+                </c:pt>
+                <c:pt idx="395">
+                  <c:v>258.12</c:v>
+                </c:pt>
+                <c:pt idx="396">
+                  <c:v>255.47</c:v>
+                </c:pt>
+                <c:pt idx="397">
+                  <c:v>248.24</c:v>
+                </c:pt>
+                <c:pt idx="398">
+                  <c:v>252.3</c:v>
+                </c:pt>
+                <c:pt idx="399">
+                  <c:v>265.12</c:v>
+                </c:pt>
+                <c:pt idx="400">
+                  <c:v>1124.6199999999999</c:v>
+                </c:pt>
+                <c:pt idx="401">
+                  <c:v>1110.04</c:v>
+                </c:pt>
+                <c:pt idx="402">
+                  <c:v>1390.72</c:v>
+                </c:pt>
+                <c:pt idx="403">
+                  <c:v>1458.31</c:v>
+                </c:pt>
+                <c:pt idx="404">
+                  <c:v>1596.93</c:v>
+                </c:pt>
+                <c:pt idx="405">
+                  <c:v>1598.85</c:v>
+                </c:pt>
+                <c:pt idx="406">
+                  <c:v>1600.48</c:v>
+                </c:pt>
+                <c:pt idx="407">
+                  <c:v>1465.96</c:v>
+                </c:pt>
+                <c:pt idx="408">
+                  <c:v>1564.04</c:v>
+                </c:pt>
+                <c:pt idx="409">
+                  <c:v>1516.91</c:v>
+                </c:pt>
+                <c:pt idx="410">
+                  <c:v>1354.57</c:v>
+                </c:pt>
+                <c:pt idx="411">
+                  <c:v>1320.33</c:v>
+                </c:pt>
+                <c:pt idx="412">
+                  <c:v>1243.07</c:v>
+                </c:pt>
+                <c:pt idx="413">
+                  <c:v>1168.45</c:v>
+                </c:pt>
+                <c:pt idx="414">
+                  <c:v>1079.1400000000001</c:v>
+                </c:pt>
+                <c:pt idx="415">
+                  <c:v>760.32</c:v>
+                </c:pt>
+                <c:pt idx="416">
+                  <c:v>486.38</c:v>
+                </c:pt>
+                <c:pt idx="417">
+                  <c:v>399.36</c:v>
+                </c:pt>
+                <c:pt idx="418">
+                  <c:v>353.07</c:v>
+                </c:pt>
+                <c:pt idx="419">
+                  <c:v>271.81</c:v>
+                </c:pt>
+                <c:pt idx="420">
+                  <c:v>264.10000000000002</c:v>
+                </c:pt>
+                <c:pt idx="421">
+                  <c:v>258.56</c:v>
+                </c:pt>
+                <c:pt idx="422">
+                  <c:v>256.35000000000002</c:v>
+                </c:pt>
+                <c:pt idx="423">
+                  <c:v>270.5</c:v>
+                </c:pt>
+                <c:pt idx="424">
+                  <c:v>1171.68</c:v>
+                </c:pt>
+                <c:pt idx="425">
+                  <c:v>1444.73</c:v>
+                </c:pt>
+                <c:pt idx="426">
+                  <c:v>1585.7</c:v>
+                </c:pt>
+                <c:pt idx="427">
+                  <c:v>1612.7</c:v>
+                </c:pt>
+                <c:pt idx="428">
+                  <c:v>1613.26</c:v>
+                </c:pt>
+                <c:pt idx="429">
+                  <c:v>1626.06</c:v>
+                </c:pt>
+                <c:pt idx="430">
+                  <c:v>1630.35</c:v>
+                </c:pt>
+                <c:pt idx="431">
+                  <c:v>1640.75</c:v>
+                </c:pt>
+                <c:pt idx="432">
+                  <c:v>1643.86</c:v>
+                </c:pt>
+                <c:pt idx="433">
+                  <c:v>1606.53</c:v>
+                </c:pt>
+                <c:pt idx="434">
+                  <c:v>1463.31</c:v>
+                </c:pt>
+                <c:pt idx="435">
+                  <c:v>1407.14</c:v>
+                </c:pt>
+                <c:pt idx="436">
+                  <c:v>1406.75</c:v>
+                </c:pt>
+                <c:pt idx="437">
+                  <c:v>1219.06</c:v>
+                </c:pt>
+                <c:pt idx="438">
+                  <c:v>1182.18</c:v>
+                </c:pt>
+                <c:pt idx="439">
+                  <c:v>1145.8800000000001</c:v>
+                </c:pt>
+                <c:pt idx="440">
+                  <c:v>1126.93</c:v>
+                </c:pt>
+                <c:pt idx="441">
+                  <c:v>999.56</c:v>
+                </c:pt>
+                <c:pt idx="442">
+                  <c:v>949.64</c:v>
+                </c:pt>
+                <c:pt idx="443">
+                  <c:v>561.48</c:v>
+                </c:pt>
+                <c:pt idx="444">
+                  <c:v>271.19</c:v>
+                </c:pt>
+                <c:pt idx="445">
+                  <c:v>271.23</c:v>
+                </c:pt>
+                <c:pt idx="446">
+                  <c:v>267.45999999999998</c:v>
+                </c:pt>
+                <c:pt idx="447">
+                  <c:v>331.37</c:v>
+                </c:pt>
+                <c:pt idx="448">
+                  <c:v>1279.72</c:v>
+                </c:pt>
+                <c:pt idx="449">
+                  <c:v>1473.73</c:v>
+                </c:pt>
+                <c:pt idx="450">
+                  <c:v>1583.82</c:v>
+                </c:pt>
+                <c:pt idx="451">
+                  <c:v>1621.92</c:v>
+                </c:pt>
+                <c:pt idx="452">
+                  <c:v>1620.4</c:v>
+                </c:pt>
+                <c:pt idx="453">
+                  <c:v>1639.78</c:v>
+                </c:pt>
+                <c:pt idx="454">
+                  <c:v>1692.45</c:v>
+                </c:pt>
+                <c:pt idx="455">
+                  <c:v>1703.23</c:v>
+                </c:pt>
+                <c:pt idx="456">
+                  <c:v>1749.7</c:v>
+                </c:pt>
+                <c:pt idx="457">
+                  <c:v>1747.59</c:v>
+                </c:pt>
+                <c:pt idx="458">
+                  <c:v>1602.82</c:v>
+                </c:pt>
+                <c:pt idx="459">
+                  <c:v>1459.92</c:v>
+                </c:pt>
+                <c:pt idx="460">
+                  <c:v>1434.26</c:v>
+                </c:pt>
+                <c:pt idx="461">
+                  <c:v>1365.36</c:v>
+                </c:pt>
+                <c:pt idx="462">
+                  <c:v>1362.97</c:v>
+                </c:pt>
+                <c:pt idx="463">
+                  <c:v>1316</c:v>
+                </c:pt>
+                <c:pt idx="464">
+                  <c:v>1272.02</c:v>
+                </c:pt>
+                <c:pt idx="465">
+                  <c:v>1169.5899999999999</c:v>
+                </c:pt>
+                <c:pt idx="466">
+                  <c:v>1066.8</c:v>
+                </c:pt>
+                <c:pt idx="467">
+                  <c:v>709.08</c:v>
+                </c:pt>
+                <c:pt idx="468">
+                  <c:v>327.33999999999997</c:v>
+                </c:pt>
+                <c:pt idx="469">
+                  <c:v>280.64999999999998</c:v>
+                </c:pt>
+                <c:pt idx="470">
+                  <c:v>299.52</c:v>
+                </c:pt>
+                <c:pt idx="471">
+                  <c:v>323.97000000000003</c:v>
+                </c:pt>
+                <c:pt idx="472">
+                  <c:v>1293.42</c:v>
+                </c:pt>
+                <c:pt idx="473">
+                  <c:v>1626.64</c:v>
+                </c:pt>
+                <c:pt idx="474">
+                  <c:v>1768.24</c:v>
+                </c:pt>
+                <c:pt idx="475">
+                  <c:v>1827.07</c:v>
+                </c:pt>
+                <c:pt idx="476">
+                  <c:v>1871.53</c:v>
+                </c:pt>
+                <c:pt idx="477">
+                  <c:v>1975.09</c:v>
+                </c:pt>
+                <c:pt idx="478">
+                  <c:v>2365.0300000000002</c:v>
+                </c:pt>
+                <c:pt idx="479">
+                  <c:v>2699.65</c:v>
+                </c:pt>
+                <c:pt idx="480">
+                  <c:v>2613.14</c:v>
+                </c:pt>
+                <c:pt idx="481">
+                  <c:v>2527.3000000000002</c:v>
+                </c:pt>
+                <c:pt idx="482">
+                  <c:v>2387.21</c:v>
+                </c:pt>
+                <c:pt idx="483">
+                  <c:v>2101.12</c:v>
+                </c:pt>
+                <c:pt idx="484">
+                  <c:v>1913.05</c:v>
+                </c:pt>
+                <c:pt idx="485">
+                  <c:v>1795.84</c:v>
+                </c:pt>
+                <c:pt idx="486">
+                  <c:v>1319.94</c:v>
+                </c:pt>
+                <c:pt idx="487">
+                  <c:v>1258.19</c:v>
+                </c:pt>
+                <c:pt idx="488">
+                  <c:v>1192.8699999999999</c:v>
+                </c:pt>
+                <c:pt idx="489">
+                  <c:v>1101.1600000000001</c:v>
+                </c:pt>
+                <c:pt idx="490">
+                  <c:v>1013.51</c:v>
+                </c:pt>
+                <c:pt idx="491">
+                  <c:v>395.94</c:v>
+                </c:pt>
+                <c:pt idx="492">
+                  <c:v>306.85000000000002</c:v>
+                </c:pt>
+                <c:pt idx="493">
+                  <c:v>310.89</c:v>
+                </c:pt>
+                <c:pt idx="494">
+                  <c:v>320.45</c:v>
+                </c:pt>
+                <c:pt idx="495">
+                  <c:v>402.78</c:v>
+                </c:pt>
+                <c:pt idx="496">
+                  <c:v>1383</c:v>
+                </c:pt>
+                <c:pt idx="497">
+                  <c:v>1650.18</c:v>
+                </c:pt>
+                <c:pt idx="498">
+                  <c:v>1776.35</c:v>
+                </c:pt>
+                <c:pt idx="499">
+                  <c:v>1814.65</c:v>
+                </c:pt>
+                <c:pt idx="500">
+                  <c:v>1802.88</c:v>
+                </c:pt>
+                <c:pt idx="501">
+                  <c:v>1836.14</c:v>
+                </c:pt>
+                <c:pt idx="502">
+                  <c:v>1834.97</c:v>
+                </c:pt>
+                <c:pt idx="503">
+                  <c:v>1831.13</c:v>
+                </c:pt>
+                <c:pt idx="504">
+                  <c:v>1879.73</c:v>
+                </c:pt>
+                <c:pt idx="505">
+                  <c:v>1879.64</c:v>
+                </c:pt>
+                <c:pt idx="506">
+                  <c:v>1716.92</c:v>
+                </c:pt>
+                <c:pt idx="507">
+                  <c:v>1536.36</c:v>
+                </c:pt>
+                <c:pt idx="508">
+                  <c:v>1431.08</c:v>
+                </c:pt>
+                <c:pt idx="509">
+                  <c:v>1353.09</c:v>
+                </c:pt>
+                <c:pt idx="510">
+                  <c:v>1278.6400000000001</c:v>
+                </c:pt>
+                <c:pt idx="511">
+                  <c:v>1205.21</c:v>
+                </c:pt>
+                <c:pt idx="512">
+                  <c:v>1153.48</c:v>
+                </c:pt>
+                <c:pt idx="513">
+                  <c:v>1067.96</c:v>
+                </c:pt>
+                <c:pt idx="514">
+                  <c:v>929.57</c:v>
+                </c:pt>
+                <c:pt idx="515">
+                  <c:v>828.92</c:v>
+                </c:pt>
+                <c:pt idx="516">
+                  <c:v>858.64</c:v>
+                </c:pt>
+                <c:pt idx="517">
+                  <c:v>832.45</c:v>
+                </c:pt>
+                <c:pt idx="518">
+                  <c:v>810.3</c:v>
+                </c:pt>
+                <c:pt idx="519">
+                  <c:v>425.57</c:v>
+                </c:pt>
+                <c:pt idx="520">
+                  <c:v>1305.74</c:v>
+                </c:pt>
+                <c:pt idx="521">
+                  <c:v>1491.53</c:v>
+                </c:pt>
+                <c:pt idx="522">
+                  <c:v>1706.32</c:v>
+                </c:pt>
+                <c:pt idx="523">
+                  <c:v>1727.84</c:v>
+                </c:pt>
+                <c:pt idx="524">
+                  <c:v>1749.63</c:v>
+                </c:pt>
+                <c:pt idx="525">
+                  <c:v>1723.05</c:v>
+                </c:pt>
+                <c:pt idx="526">
+                  <c:v>1733.63</c:v>
+                </c:pt>
+                <c:pt idx="527">
+                  <c:v>1798.02</c:v>
+                </c:pt>
+                <c:pt idx="528">
+                  <c:v>1859.21</c:v>
+                </c:pt>
+                <c:pt idx="529">
+                  <c:v>1814.28</c:v>
+                </c:pt>
+                <c:pt idx="530">
+                  <c:v>1562.55</c:v>
+                </c:pt>
+                <c:pt idx="531">
+                  <c:v>1539.43</c:v>
+                </c:pt>
+                <c:pt idx="532">
+                  <c:v>1474.61</c:v>
+                </c:pt>
+                <c:pt idx="533">
+                  <c:v>1413.76</c:v>
+                </c:pt>
+                <c:pt idx="534">
+                  <c:v>1360.37</c:v>
+                </c:pt>
+                <c:pt idx="535">
+                  <c:v>1309.24</c:v>
+                </c:pt>
+                <c:pt idx="536">
+                  <c:v>1249.23</c:v>
+                </c:pt>
+                <c:pt idx="537">
+                  <c:v>1164.08</c:v>
+                </c:pt>
+                <c:pt idx="538">
+                  <c:v>1113.42</c:v>
+                </c:pt>
+                <c:pt idx="539">
+                  <c:v>964.61</c:v>
+                </c:pt>
+                <c:pt idx="540">
+                  <c:v>938.91</c:v>
+                </c:pt>
+                <c:pt idx="541">
+                  <c:v>935.71</c:v>
+                </c:pt>
+                <c:pt idx="542">
+                  <c:v>934.84</c:v>
+                </c:pt>
+                <c:pt idx="543">
+                  <c:v>960.76</c:v>
+                </c:pt>
+                <c:pt idx="544">
+                  <c:v>1281.6400000000001</c:v>
+                </c:pt>
+                <c:pt idx="545">
+                  <c:v>1580.62</c:v>
+                </c:pt>
+                <c:pt idx="546">
+                  <c:v>1708.62</c:v>
+                </c:pt>
+                <c:pt idx="547">
+                  <c:v>1741.26</c:v>
+                </c:pt>
+                <c:pt idx="548">
+                  <c:v>1800.69</c:v>
+                </c:pt>
+                <c:pt idx="549">
+                  <c:v>1781.15</c:v>
+                </c:pt>
+                <c:pt idx="550">
+                  <c:v>1792.21</c:v>
+                </c:pt>
+                <c:pt idx="551">
+                  <c:v>1863.08</c:v>
+                </c:pt>
+                <c:pt idx="552">
+                  <c:v>1872.17</c:v>
+                </c:pt>
+                <c:pt idx="553">
+                  <c:v>1851.33</c:v>
+                </c:pt>
+                <c:pt idx="554">
+                  <c:v>1725.79</c:v>
+                </c:pt>
+                <c:pt idx="555">
+                  <c:v>1581.09</c:v>
+                </c:pt>
+                <c:pt idx="556">
+                  <c:v>1490.02</c:v>
+                </c:pt>
+                <c:pt idx="557">
+                  <c:v>1468.29</c:v>
+                </c:pt>
+                <c:pt idx="558">
+                  <c:v>1435.18</c:v>
+                </c:pt>
+                <c:pt idx="559">
+                  <c:v>1367.93</c:v>
+                </c:pt>
+                <c:pt idx="560">
+                  <c:v>1317.9</c:v>
+                </c:pt>
+                <c:pt idx="561">
+                  <c:v>1205.01</c:v>
+                </c:pt>
+                <c:pt idx="562">
+                  <c:v>1121.58</c:v>
+                </c:pt>
+                <c:pt idx="563">
+                  <c:v>1010.27</c:v>
+                </c:pt>
+                <c:pt idx="564">
+                  <c:v>988.2</c:v>
+                </c:pt>
+                <c:pt idx="565">
+                  <c:v>955.22</c:v>
+                </c:pt>
+                <c:pt idx="566">
+                  <c:v>947.95</c:v>
+                </c:pt>
+                <c:pt idx="567">
+                  <c:v>1003.91</c:v>
+                </c:pt>
+                <c:pt idx="568">
+                  <c:v>1139.8399999999999</c:v>
+                </c:pt>
+                <c:pt idx="569">
+                  <c:v>1314.43</c:v>
+                </c:pt>
+                <c:pt idx="570">
+                  <c:v>1457.04</c:v>
+                </c:pt>
+                <c:pt idx="571">
+                  <c:v>1477.34</c:v>
+                </c:pt>
+                <c:pt idx="572">
+                  <c:v>1484.18</c:v>
+                </c:pt>
+                <c:pt idx="573">
+                  <c:v>1445.81</c:v>
+                </c:pt>
+                <c:pt idx="574">
+                  <c:v>1471.5</c:v>
+                </c:pt>
+                <c:pt idx="575">
+                  <c:v>1490.92</c:v>
+                </c:pt>
+                <c:pt idx="576">
+                  <c:v>1463.16</c:v>
+                </c:pt>
+                <c:pt idx="577">
+                  <c:v>1439.97</c:v>
+                </c:pt>
+                <c:pt idx="578">
+                  <c:v>1332.98</c:v>
+                </c:pt>
+                <c:pt idx="579">
+                  <c:v>1254.5</c:v>
+                </c:pt>
+                <c:pt idx="580">
+                  <c:v>1183.52</c:v>
+                </c:pt>
+                <c:pt idx="581">
+                  <c:v>1159.48</c:v>
+                </c:pt>
+                <c:pt idx="582">
+                  <c:v>1118.3</c:v>
+                </c:pt>
+                <c:pt idx="583">
+                  <c:v>1127.3</c:v>
+                </c:pt>
+                <c:pt idx="584">
+                  <c:v>1095.2</c:v>
+                </c:pt>
+                <c:pt idx="585">
+                  <c:v>1024.43</c:v>
+                </c:pt>
+                <c:pt idx="586">
+                  <c:v>978.02</c:v>
+                </c:pt>
+                <c:pt idx="587">
+                  <c:v>887.86</c:v>
+                </c:pt>
+                <c:pt idx="588">
+                  <c:v>875.38</c:v>
+                </c:pt>
+                <c:pt idx="589">
+                  <c:v>897.07</c:v>
+                </c:pt>
+                <c:pt idx="590">
+                  <c:v>883.02</c:v>
+                </c:pt>
+                <c:pt idx="591">
+                  <c:v>912.31</c:v>
+                </c:pt>
+                <c:pt idx="592">
+                  <c:v>1162.76</c:v>
+                </c:pt>
+                <c:pt idx="593">
+                  <c:v>1295.76</c:v>
+                </c:pt>
+                <c:pt idx="594">
+                  <c:v>1352.58</c:v>
+                </c:pt>
+                <c:pt idx="595">
+                  <c:v>1399.28</c:v>
+                </c:pt>
+                <c:pt idx="596">
+                  <c:v>1408.64</c:v>
+                </c:pt>
+                <c:pt idx="597">
+                  <c:v>1388.93</c:v>
+                </c:pt>
+                <c:pt idx="598">
+                  <c:v>1383.94</c:v>
+                </c:pt>
+                <c:pt idx="599">
+                  <c:v>1369.11</c:v>
+                </c:pt>
+                <c:pt idx="600">
+                  <c:v>1394.02</c:v>
+                </c:pt>
+                <c:pt idx="601">
+                  <c:v>1298.1400000000001</c:v>
+                </c:pt>
+                <c:pt idx="602">
+                  <c:v>1185.3599999999999</c:v>
+                </c:pt>
+                <c:pt idx="603">
+                  <c:v>1093.46</c:v>
+                </c:pt>
+                <c:pt idx="604">
+                  <c:v>1048.9100000000001</c:v>
+                </c:pt>
+                <c:pt idx="605">
+                  <c:v>1006.38</c:v>
+                </c:pt>
+                <c:pt idx="606">
+                  <c:v>1001.19</c:v>
+                </c:pt>
+                <c:pt idx="607">
+                  <c:v>979.68</c:v>
+                </c:pt>
+                <c:pt idx="608">
+                  <c:v>950.29</c:v>
+                </c:pt>
+                <c:pt idx="609">
+                  <c:v>896.16</c:v>
+                </c:pt>
+                <c:pt idx="610">
+                  <c:v>853.87</c:v>
+                </c:pt>
+                <c:pt idx="611">
+                  <c:v>767.6</c:v>
+                </c:pt>
+                <c:pt idx="612">
+                  <c:v>754.23</c:v>
+                </c:pt>
+                <c:pt idx="613">
+                  <c:v>745.77</c:v>
+                </c:pt>
+                <c:pt idx="614">
+                  <c:v>743.19</c:v>
+                </c:pt>
+                <c:pt idx="615">
+                  <c:v>763.1</c:v>
+                </c:pt>
+                <c:pt idx="616">
+                  <c:v>1083.08</c:v>
+                </c:pt>
+                <c:pt idx="617">
+                  <c:v>1508.99</c:v>
+                </c:pt>
+                <c:pt idx="618">
+                  <c:v>1663.3</c:v>
+                </c:pt>
+                <c:pt idx="619">
+                  <c:v>1718.9</c:v>
+                </c:pt>
+                <c:pt idx="620">
+                  <c:v>1757.25</c:v>
+                </c:pt>
+                <c:pt idx="621">
+                  <c:v>1728.1</c:v>
+                </c:pt>
+                <c:pt idx="622">
+                  <c:v>1782.97</c:v>
+                </c:pt>
+                <c:pt idx="623">
+                  <c:v>1789.95</c:v>
+                </c:pt>
+                <c:pt idx="624">
+                  <c:v>1840.16</c:v>
+                </c:pt>
+                <c:pt idx="625">
+                  <c:v>1837.25</c:v>
+                </c:pt>
+                <c:pt idx="626">
+                  <c:v>1733.39</c:v>
+                </c:pt>
+                <c:pt idx="627">
+                  <c:v>1572.53</c:v>
+                </c:pt>
+                <c:pt idx="628">
+                  <c:v>1449.66</c:v>
+                </c:pt>
+                <c:pt idx="629">
+                  <c:v>1342.26</c:v>
+                </c:pt>
+                <c:pt idx="630">
+                  <c:v>1227.29</c:v>
+                </c:pt>
+                <c:pt idx="631">
+                  <c:v>1196.32</c:v>
+                </c:pt>
+                <c:pt idx="632">
+                  <c:v>1150.08</c:v>
+                </c:pt>
+                <c:pt idx="633">
+                  <c:v>1088.5</c:v>
+                </c:pt>
+                <c:pt idx="634">
+                  <c:v>1023.9</c:v>
+                </c:pt>
+                <c:pt idx="635">
+                  <c:v>906.02</c:v>
+                </c:pt>
+                <c:pt idx="636">
+                  <c:v>884.59</c:v>
+                </c:pt>
+                <c:pt idx="637">
+                  <c:v>889.18</c:v>
+                </c:pt>
+                <c:pt idx="638">
+                  <c:v>886.3</c:v>
+                </c:pt>
+                <c:pt idx="639">
+                  <c:v>913.7</c:v>
+                </c:pt>
+                <c:pt idx="640">
+                  <c:v>1261.1400000000001</c:v>
+                </c:pt>
+                <c:pt idx="641">
+                  <c:v>1543.74</c:v>
+                </c:pt>
+                <c:pt idx="642">
+                  <c:v>1710.99</c:v>
+                </c:pt>
+                <c:pt idx="643">
+                  <c:v>1774.05</c:v>
+                </c:pt>
+                <c:pt idx="644">
+                  <c:v>1818.66</c:v>
+                </c:pt>
+                <c:pt idx="645">
+                  <c:v>1819.66</c:v>
+                </c:pt>
+                <c:pt idx="646">
+                  <c:v>1837.72</c:v>
+                </c:pt>
+                <c:pt idx="647">
+                  <c:v>1861.39</c:v>
+                </c:pt>
+                <c:pt idx="648">
+                  <c:v>1923.83</c:v>
+                </c:pt>
+                <c:pt idx="649">
+                  <c:v>1894.61</c:v>
+                </c:pt>
+                <c:pt idx="650">
+                  <c:v>1762.51</c:v>
+                </c:pt>
+                <c:pt idx="651">
+                  <c:v>1602.37</c:v>
+                </c:pt>
+                <c:pt idx="652">
+                  <c:v>1515.12</c:v>
+                </c:pt>
+                <c:pt idx="653">
+                  <c:v>1432.2</c:v>
+                </c:pt>
+                <c:pt idx="654">
+                  <c:v>1284.78</c:v>
+                </c:pt>
+                <c:pt idx="655">
+                  <c:v>1267.07</c:v>
+                </c:pt>
+                <c:pt idx="656">
+                  <c:v>1203.5899999999999</c:v>
+                </c:pt>
+                <c:pt idx="657">
+                  <c:v>1128.01</c:v>
+                </c:pt>
+                <c:pt idx="658">
+                  <c:v>1031.6199999999999</c:v>
+                </c:pt>
+                <c:pt idx="659">
+                  <c:v>909.8</c:v>
+                </c:pt>
+                <c:pt idx="660">
+                  <c:v>872.82</c:v>
+                </c:pt>
+                <c:pt idx="661">
+                  <c:v>882.19</c:v>
+                </c:pt>
+                <c:pt idx="662">
+                  <c:v>842.88</c:v>
+                </c:pt>
+                <c:pt idx="663">
+                  <c:v>879.5</c:v>
+                </c:pt>
+                <c:pt idx="664">
+                  <c:v>1184.8699999999999</c:v>
+                </c:pt>
+                <c:pt idx="665">
+                  <c:v>1476.67</c:v>
+                </c:pt>
+                <c:pt idx="666">
+                  <c:v>1609.32</c:v>
+                </c:pt>
+                <c:pt idx="667">
+                  <c:v>1685.03</c:v>
+                </c:pt>
+                <c:pt idx="668">
+                  <c:v>1740.17</c:v>
+                </c:pt>
+                <c:pt idx="669">
+                  <c:v>1735.85</c:v>
+                </c:pt>
+                <c:pt idx="670">
+                  <c:v>1769.37</c:v>
+                </c:pt>
+                <c:pt idx="671">
+                  <c:v>1832.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D8AC-4876-A8DD-7A11B4F01AEE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="319052255"/>
+        <c:axId val="319051839"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="319052255"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="319051839"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="319051839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="319052255"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>663</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>702</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87507095-F056-725E-5084-4CB4E6A36F74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2423,8 +7339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B688"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A656" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A675" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:B688"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -7941,5 +12857,6 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>